<commit_message>
race strat table and small corrections
</commit_message>
<xml_diff>
--- a/Manuscript_items/ARIC_table.xlsx
+++ b/Manuscript_items/ARIC_table.xlsx
@@ -407,7 +407,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="B2">
@@ -500,7 +500,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="B5">
@@ -593,7 +593,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="B8">
@@ -686,7 +686,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="B11">
@@ -779,7 +779,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="B14">
@@ -872,7 +872,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Combined</t>
         </is>
       </c>
       <c r="B17">

</xml_diff>